<commit_message>
Ajout d'un vol terminé, affichage pilote
</commit_message>
<xml_diff>
--- a/Documentation/Tests unitaire/Tests unitaires.xlsx
+++ b/Documentation/Tests unitaire/Tests unitaires.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="44">
   <si>
     <t>Comportement Observé</t>
   </si>
@@ -100,6 +100,57 @@
   </si>
   <si>
     <t>Si le lieu de départ et/ou le lieu d'arrivée ne sont pas sélectionnés, message d'avertissement                                                       Si le lieu de départ correspond au lieu d'arrivée, message d'avertissement                                                                                                     Si la distance n'est pas rentrée, message d'avertissement    Si la distance commence par 0, message d'avertissement    Si tous les champs sont remplis correctement deux lignes sont crées (Ligne allé = ArrivalAirport-DepartureAirport, ligne retour DepartureAirport-ArrivalAirport)</t>
+  </si>
+  <si>
+    <t>Ajout d'un vol</t>
+  </si>
+  <si>
+    <t>Date de départ</t>
+  </si>
+  <si>
+    <t>Lorsque je sélectionne une date grâce au dateTimePicker, la date sélectionnée s'affiche comme étant la date sélectionnée</t>
+  </si>
+  <si>
+    <t>La date s'affiche correctement</t>
+  </si>
+  <si>
+    <t>Heure de départ</t>
+  </si>
+  <si>
+    <t>Lorsque je clique sur les flèches du numericUpDown, la valeur du numericUpDown s'incrémente ou se décrémente</t>
+  </si>
+  <si>
+    <t>La valeur du numericUpDown se décrémente ou s'incrémente correctement</t>
+  </si>
+  <si>
+    <t>Ligne</t>
+  </si>
+  <si>
+    <t>Lorsque je sélectionne une ligne grâce à la combobox la ligne sélectionnée s'affiche comment étant la ligne sélectionnée</t>
+  </si>
+  <si>
+    <t>La ligne s'affiche correctement</t>
+  </si>
+  <si>
+    <t>Voir date arrivée</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lorsque je clique sur le bouton  :                                           Si aucune ligne n'a été sélectionnée, message d'avertissement                                                                                   Si la date de départ est celle du jour, message de confirmation pour être sûr que c'est bien la date voulue                                                                                                         Si l'heure de départ est à 0:0, message de confimration pour être sûr que c'est bien l'heure voulue                                                                                                        Si tous les champs sont renseignés, enable le bouton ajouter                                                                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Si aucune ligne n'a été sélectionnée, message d'avertissement                                                                                   Si la date de départ est celle du jour, message de confirmation pour être sûr que c'est bien la date voulue                                                                                                         Si l'heure de départ est à 0:0, message de confimration pour être sûr que c'est bien l'heure voulue                                                                                                        Si tous les champs sont renseignés, enable le bouton ajouter       </t>
+  </si>
+  <si>
+    <t>"Modification d'un champ"</t>
+  </si>
+  <si>
+    <t>Si un champ est modifié après avoir appuyé sur le bouton "Voir date d'arrivée", le bouton "Ajouter" devient disable</t>
+  </si>
+  <si>
+    <t>Lorsque je clique sur le bouton, un vol est ajouté dans la base de données et un message averti l'utilisateur que le vol a été ajouté</t>
+  </si>
+  <si>
+    <t>un vol est ajouté dans la base de données et un message averti l'utilisateur que le vol a été ajouté</t>
   </si>
 </sst>
 </file>
@@ -129,7 +180,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -154,6 +205,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -167,7 +224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -182,6 +239,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -463,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,13 +630,12 @@
       <c r="A8" s="4"/>
       <c r="B8" s="3"/>
       <c r="C8" s="4"/>
-      <c r="D8" s="5"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="3"/>
       <c r="C9" s="4"/>
-      <c r="D9" s="5"/>
+      <c r="D9" s="7"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
@@ -650,6 +709,109 @@
         <v>26</v>
       </c>
       <c r="D17" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="165" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" s="5" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Ajout des vacances - pas terminé
</commit_message>
<xml_diff>
--- a/Documentation/Tests unitaire/Tests unitaires.xlsx
+++ b/Documentation/Tests unitaire/Tests unitaires.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="54">
   <si>
     <t>Comportement Observé</t>
   </si>
@@ -151,6 +151,36 @@
   </si>
   <si>
     <t>un vol est ajouté dans la base de données et un message averti l'utilisateur que le vol a été ajouté</t>
+  </si>
+  <si>
+    <t>Affichage d'un pilote</t>
+  </si>
+  <si>
+    <t>DataGridViewer</t>
+  </si>
+  <si>
+    <t>Les informations sont retrouvées dans les cases correspondantes du dataGridView pour chaque pilote</t>
+  </si>
+  <si>
+    <t>Affichage d'un vol</t>
+  </si>
+  <si>
+    <t>Pour chaque vol répertorié dans la base de données sont affichées par ligne les informations suivantes : Nom, Ligne, Date départ, Date arrivée, Pilot n°1, Pilote n°2</t>
+  </si>
+  <si>
+    <t>Les informations sont retrouvées dans les cases correspondantes du dataGridView pour chaque vol. Mais comme l'affectation d'un vol à un pilote n'est pas encore implémantée, je ne peux pas verifier si l'information est correcte pour Pilote n°1 et Pilote n°2</t>
+  </si>
+  <si>
+    <t>Affichage d'une ligne</t>
+  </si>
+  <si>
+    <t>Pour chaque pilote répertorié dans la base de données sont affichées par ligne les informations suivantes : Id, Nom, Prénom, Aéroport d'affectation, Heures de vol</t>
+  </si>
+  <si>
+    <t>Pour chaque ligne répertoriée dans la base de données sont affichées par ligne les informations suivantes : Id, lieu de départ, lieu d'arrivée, distance</t>
+  </si>
+  <si>
+    <t>Les informations sont retrouvées dans les cases correspondantes du dataGridView pour chaque ligne</t>
   </si>
 </sst>
 </file>
@@ -523,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -815,6 +845,105 @@
         <v>2</v>
       </c>
     </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Ajout vacances - affichage vacances
</commit_message>
<xml_diff>
--- a/Documentation/Tests unitaire/Tests unitaires.xlsx
+++ b/Documentation/Tests unitaire/Tests unitaires.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="67">
   <si>
     <t>Comportement Observé</t>
   </si>
@@ -181,6 +181,45 @@
   </si>
   <si>
     <t>Les informations sont retrouvées dans les cases correspondantes du dataGridView pour chaque ligne</t>
+  </si>
+  <si>
+    <t>Planification vacances</t>
+  </si>
+  <si>
+    <t>Si aucune ligne n'est sélectionnée dans le DataGridView, message d'avertissement                               Si toutes les lignes sont sélectionnées dans le DataGridView, message d'avertissement                                Si une ligne est sélectionnée et que le pilote a deja ses 25jours de vacances, message d'avertissement      Si une ligne est sélectionnée et que le pilote a encore des jours de vacances disponbiles, le formulaire frmVacances s'ouvre</t>
+  </si>
+  <si>
+    <t>Si aucune ligne n'est sélectionnée dans le DataGridView, message d'avertissement                                                                Si toutes les lignes sont sélectionnées dans le DataGridView, message d'avertissement                                  Si une ligne est sélectionnée et que le pilote a deja ses 25jours de vacances, message d'avertissement                     Si une ligne est sélectionnée et que le pilote a encore des jours de vacances disponbiles, le formulaire frmVacances s'ouvre</t>
+  </si>
+  <si>
+    <t>Valider (frmVacances)</t>
+  </si>
+  <si>
+    <t>Si la date de début précède le jour même, message d'avertissement                                                                                         Si la date de fin précède la date de début, message d'avertissement                                                                                Si le nombre de jours que l'on veut ajouter dépasse le nombre de jours de vacances restant au pilote, message d'avertissement                                                               Si la date de débout ou la date de fin correspondent a une date de vacances deja existante du pilote, message d'avertissement                                                                  Si la date de début et la date de fin sont "correctes", les vacances sont ajoutées dans la base de données, message d'avertissement</t>
+  </si>
+  <si>
+    <t>Si la date de début précède le jour même, message d'avertissement                                                                                         Si la date de fin précède la date de début, message d'avertissement                                                                                    Si le nombre de jours que l'on veut ajouter dépasse le nombre de jours de vacances restant au pilote, message d'avertissement                                                                                    Si la date de débout ou la date de fin correspondent a une date de vacances deja existante du pilote, message d'avertissement                                                                                              Si la date de début et la date de fin sont "correctes", les vacances sont ajoutées dans la base de données, message d'avertissement</t>
+  </si>
+  <si>
+    <t>Affichage vacances</t>
+  </si>
+  <si>
+    <t>Planifier les vacances</t>
+  </si>
+  <si>
+    <t>Afficher les vacances</t>
+  </si>
+  <si>
+    <t>Si aucune ligne n'est sélectionnée dans le DataGridView, message d'avertissement                               Si toutes les lignes sont sélectionnées dans le DataGridView, message d'avertissement                              Si une seule ligne est sélectionnée, le formualire frmVacancesAffichage s'ouvre</t>
+  </si>
+  <si>
+    <t>Si aucune ligne n'est sélectionnée dans le DataGridView, message d'avertissement                                                                              Si toutes les lignes sont sélectionnées dans le DataGridView, message d'avertissement                                                  Si une seule ligne est sélectionnée, le formualire frmVacancesAffichage s'ouvre</t>
+  </si>
+  <si>
+    <t>frmVacancesAffichage.Load()</t>
+  </si>
+  <si>
+    <t>Toutes les vacances du pilote sélectionné s'affichent</t>
   </si>
 </sst>
 </file>
@@ -242,7 +281,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -250,11 +289,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -273,6 +327,7 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -553,10 +608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -944,6 +999,115 @@
         <v>2</v>
       </c>
     </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="195" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="4"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="6"/>
+      <c r="D51" s="7"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="4"/>
+      <c r="B52" s="3"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="7"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D57" s="8"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Affectation d'un pilote a un vol (non terminé) - Gestion planing (non terminé)
</commit_message>
<xml_diff>
--- a/Documentation/Tests unitaire/Tests unitaires.xlsx
+++ b/Documentation/Tests unitaire/Tests unitaires.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="90">
   <si>
     <t>Comportement Observé</t>
   </si>
@@ -63,9 +63,6 @@
     <t>Ajouter</t>
   </si>
   <si>
-    <t>Lorsque je clique sur ajouter si : un ou des champs ne sont pas remplis  -&gt; message d'avertissement; un champ ne contient pas les caractères adaptés à ce champ -&gt; message d'avertissement; le nom ou le prénom dépasse les 45 caractères -&gt; messages d'avertissement; si les heures de vols commencent par 0 -&gt; message d'avertissement. Si tous les champs sont remplis correctement un pilote est ajouté dans la base de données</t>
-  </si>
-  <si>
     <t>Si le nom ou le prénom contiennent autres choses que des lettres, message d'avertissement                                              Si le nom ou le prénom font plus de 45 caractères, message d'avertissement                                                                               Si les heures de vols a son actif contiennent autres choses que des chiffres, message d'avertissement                                   Si les heures de vols à son actif commencent par 0, message d'avertissement                                                                 Si un ou plusieurs champs ne sont pas remplis, message d'avertissement                                                                                             Si tous les champs sont remplis correctement, le pilote est ajouté dans la base de données</t>
   </si>
   <si>
@@ -96,12 +93,6 @@
     <t>Le lieu d'arrivée s'affiche correctement</t>
   </si>
   <si>
-    <t>Lorsque je clique sur ajouter si: un ou des champs ne sont pas remplis -&gt; message d'avertissement, le champ distance ne contient pas que des chiffres ou commence par 0 -&gt; avertissement; le lieu d'arrivée et le meme que le lieu de départ -&gt; avertissement</t>
-  </si>
-  <si>
-    <t>Si le lieu de départ et/ou le lieu d'arrivée ne sont pas sélectionnés, message d'avertissement                                                       Si le lieu de départ correspond au lieu d'arrivée, message d'avertissement                                                                                                     Si la distance n'est pas rentrée, message d'avertissement    Si la distance commence par 0, message d'avertissement    Si tous les champs sont remplis correctement deux lignes sont crées (Ligne allé = ArrivalAirport-DepartureAirport, ligne retour DepartureAirport-ArrivalAirport)</t>
-  </si>
-  <si>
     <t>Ajout d'un vol</t>
   </si>
   <si>
@@ -147,12 +138,6 @@
     <t>Si un champ est modifié après avoir appuyé sur le bouton "Voir date d'arrivée", le bouton "Ajouter" devient disable</t>
   </si>
   <si>
-    <t>Lorsque je clique sur le bouton, un vol est ajouté dans la base de données et un message averti l'utilisateur que le vol a été ajouté</t>
-  </si>
-  <si>
-    <t>un vol est ajouté dans la base de données et un message averti l'utilisateur que le vol a été ajouté</t>
-  </si>
-  <si>
     <t>Affichage d'un pilote</t>
   </si>
   <si>
@@ -195,12 +180,6 @@
     <t>Valider (frmVacances)</t>
   </si>
   <si>
-    <t>Si la date de début précède le jour même, message d'avertissement                                                                                         Si la date de fin précède la date de début, message d'avertissement                                                                                Si le nombre de jours que l'on veut ajouter dépasse le nombre de jours de vacances restant au pilote, message d'avertissement                                                               Si la date de débout ou la date de fin correspondent a une date de vacances deja existante du pilote, message d'avertissement                                                                  Si la date de début et la date de fin sont "correctes", les vacances sont ajoutées dans la base de données, message d'avertissement</t>
-  </si>
-  <si>
-    <t>Si la date de début précède le jour même, message d'avertissement                                                                                         Si la date de fin précède la date de début, message d'avertissement                                                                                    Si le nombre de jours que l'on veut ajouter dépasse le nombre de jours de vacances restant au pilote, message d'avertissement                                                                                    Si la date de débout ou la date de fin correspondent a une date de vacances deja existante du pilote, message d'avertissement                                                                                              Si la date de début et la date de fin sont "correctes", les vacances sont ajoutées dans la base de données, message d'avertissement</t>
-  </si>
-  <si>
     <t>Affichage vacances</t>
   </si>
   <si>
@@ -216,17 +195,129 @@
     <t>Si aucune ligne n'est sélectionnée dans le DataGridView, message d'avertissement                                                                              Si toutes les lignes sont sélectionnées dans le DataGridView, message d'avertissement                                                  Si une seule ligne est sélectionnée, le formualire frmVacancesAffichage s'ouvre</t>
   </si>
   <si>
-    <t>frmVacancesAffichage.Load()</t>
-  </si>
-  <si>
     <t>Toutes les vacances du pilote sélectionné s'affichent</t>
+  </si>
+  <si>
+    <t>Affectation d'un pilote à un vol</t>
+  </si>
+  <si>
+    <t>Planifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">frmFlightAssignment_Load </t>
+  </si>
+  <si>
+    <t>frmVacancesAffichage_Load</t>
+  </si>
+  <si>
+    <t>frmFlightAssignment_Load  - LoadAllPilotsInCurrentAirport()</t>
+  </si>
+  <si>
+    <t>A l'ouverture du formulaire les actions decrites si dessous se passent</t>
+  </si>
+  <si>
+    <t>Tous les pilotes qui se trouvent dans le même aeroport que l'aeroport de départ sont ajoutés dans la liste lstAvailablePilots</t>
+  </si>
+  <si>
+    <t>frmFlightAssignment_Load  - RemovePilotsNoRestAfterFlight()</t>
+  </si>
+  <si>
+    <t>Pour chaque pilote se trouvant dans la liste, si il n'y a pas 12h d'écart entre la date du départ de ce vol et la date a laquelle le pilote a fait son dernier vol, le pilote est retiré de la liste</t>
+  </si>
+  <si>
+    <t>Si il n'y a pas les 12h d'écart, le pilote est retiré de la liste</t>
+  </si>
+  <si>
+    <t>frmFlightAssignment_Load  - RemovePilotsInVacation()</t>
+  </si>
+  <si>
+    <t>Pour chaque pilote se trouvant dans la liste, si il est en vacances à la date de ce vol, le pilote est retiré de la liste</t>
+  </si>
+  <si>
+    <t>frmFlightAssignment_Load  - RemovePilotsWorking()</t>
+  </si>
+  <si>
+    <t>Pour chaque pilote se trouvant dans la liste, si il est en train de travailler à la date du vol, il est retiré de la liste</t>
+  </si>
+  <si>
+    <t>Si le pilote est en train de travailler à la date du vol, il est retiré de la liste</t>
+  </si>
+  <si>
+    <t>frmFlightAssignment_Load  - RemovePilotsNoRestThisWeek()</t>
+  </si>
+  <si>
+    <t>Pour chaque pilote se trouvant dans la liste, si il n'a pas eu 2 jours de repos cette semaine et si dans le cas ou il est affecté à ce vol il n'aurait pas le temps de les prendre, le pilote est retiré de la liste</t>
+  </si>
+  <si>
+    <t>La méthode n'est pas implémentée jusqu'au bout, elle est inutilisable pour l'instant.</t>
+  </si>
+  <si>
+    <t>Si le pilote est en vacance à la date du vol, il est retiré de la liste.</t>
+  </si>
+  <si>
+    <t>Tous les pilotes se trouvant dans le même aéroport que l'aéroport de départ sont bien ajoutés à la liste, cela fonctionne pour un vol imminent. Mais si le vol n'est pas tout de suite, la fonction calcule mal la localisation actuelle du pilote</t>
+  </si>
+  <si>
+    <t>OK DANS CERTAINS CAS</t>
+  </si>
+  <si>
+    <t>PAS IMPLEMENTEE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Si la date de début précède le jour même, message d'avertissement                                                                                         Si la date de fin précède la date de début, message d'avertissement                                                                                Si le nombre de jours que l'on veut ajouter dépasse le nombre de jours de vacances restant au pilote, message d'avertissement                                                               Si la date de débout ou la date de fin correspondent a une date de vacances deja existante du pilote, message d'avertissement                                                                      Si le pilote est en train de travailler pendant la periode de vacances, message d'avertissement                                                     Si la date de début et la date de fin sont "correctes", les vacances sont ajoutées dans la base de données, message d'avertissement                                                                               </t>
+  </si>
+  <si>
+    <t>OK, SAUF CAS SPECIFIQUE</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Si la date de début précède le jour même, message d'avertissement                                                                                         Si la date de fin précède la date de début, message d'avertissement                                                                                    Si le nombre de jours que l'on veut ajouter dépasse le nombre de jours de vacances restant au pilote, message d'avertissement                                                                                    Si la date de débout ou la date de fin correspondent a une date de vacances deja existante du pilote, message d'avertissement                                                                                                  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Si le pilote est en train de travailler pendant la periode de vacances, les vacances sont quand même ajoutées   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                                                                                   Si la date de début et la date de fin sont "correctes", les vacances sont ajoutées dans la base de données, message d'avertissement</t>
+    </r>
+  </si>
+  <si>
+    <t>Lorsque je clique sur ajouter si : un ou des champs ne sont pas remplis  -&gt; message d'avertissement; un champ ne contient pas les caractères adaptés à ce champ -&gt; message d'avertissement; le nom ou le prénom dépasse les 45 caractères -&gt; messages d'avertissement; si les heures de vols commencent par 0 -&gt; message d'avertissement.                                            Si tous les champs sont remplis correctement un pilote est ajouté dans la base de données</t>
+  </si>
+  <si>
+    <t>Lorsque je clique sur ajouter si: un ou des champs ne sont pas remplis -&gt; message d'avertissement, le champ distance ne contient pas que des chiffres ou commence par 0 -&gt; avertissement; le lieu d'arrivée et le meme que le lieu de départ -&gt; avertissement     Si la ligne que l'on veut ajouter existe deja, message d'avertissement</t>
+  </si>
+  <si>
+    <t>Si le lieu de départ et/ou le lieu d'arrivée ne sont pas sélectionnés, message d'avertissement                                                       Si le lieu de départ correspond au lieu d'arrivée, message d'avertissement                                                                                                     Si la distance n'est pas rentrée, message d'avertissement    Si la distance commence par 0, message d'avertissement    Il n'y a pas de vérification si la ligne existe deja                              Si tous les champs sont remplis correctement deux lignes sont crées (Ligne allé = ArrivalAirport-DepartureAirport, ligne retour DepartureAirport-ArrivalAirport)</t>
+  </si>
+  <si>
+    <t>Lorsque je clique sur le bouton, un vol est ajouté dans la base de données et un message averti l'utilisateur que le vol a été ajouté                                                Si le vol existe déjà, message d'avertissement</t>
+  </si>
+  <si>
+    <t>un vol est ajouté dans la base de données et un message averti l'utilisateur que le vol a été ajouté                                        Il n'y a pas de vérification si le vol existe déjà ou pas</t>
+  </si>
+  <si>
+    <t>OK, sauf cas spécifique</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -248,8 +339,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -277,6 +375,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -308,7 +418,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -328,6 +438,22 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -608,18 +734,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D57"/>
+  <dimension ref="A1:E68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" customWidth="1"/>
+    <col min="1" max="1" width="28.28515625" customWidth="1"/>
     <col min="2" max="2" width="47.140625" customWidth="1"/>
     <col min="3" max="3" width="51.5703125" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" customWidth="1"/>
+    <col min="5" max="5" width="58.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -688,7 +815,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>12</v>
@@ -702,10 +829,10 @@
         <v>13</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>15</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>2</v>
@@ -724,7 +851,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -743,13 +870,13 @@
     </row>
     <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>22</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>2</v>
@@ -757,13 +884,13 @@
     </row>
     <row r="15" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>24</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>2</v>
@@ -771,7 +898,7 @@
     </row>
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>7</v>
@@ -783,23 +910,23 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="165" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>25</v>
+        <v>85</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>2</v>
+        <v>86</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -818,13 +945,13 @@
     </row>
     <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>2</v>
@@ -832,13 +959,13 @@
     </row>
     <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>2</v>
@@ -846,13 +973,13 @@
     </row>
     <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>2</v>
@@ -860,13 +987,13 @@
     </row>
     <row r="25" spans="1:4" ht="165" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>2</v>
@@ -874,35 +1001,35 @@
     </row>
     <row r="26" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>42</v>
+        <v>87</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>2</v>
+        <v>88</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -921,13 +1048,13 @@
     </row>
     <row r="33" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>2</v>
@@ -935,7 +1062,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -954,13 +1081,13 @@
     </row>
     <row r="39" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>2</v>
@@ -968,7 +1095,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -987,13 +1114,13 @@
     </row>
     <row r="44" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D44" s="5" t="s">
         <v>2</v>
@@ -1001,7 +1128,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1020,30 +1147,30 @@
     </row>
     <row r="49" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D49" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="195" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" ht="225" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>2</v>
+        <v>83</v>
+      </c>
+      <c r="D50" s="14" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1060,7 +1187,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1079,13 +1206,13 @@
     </row>
     <row r="55" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D55" s="5" t="s">
         <v>2</v>
@@ -1093,13 +1220,13 @@
     </row>
     <row r="56" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D56" s="5" t="s">
         <v>2</v>
@@ -1107,6 +1234,118 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D57" s="8"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D64" s="11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D65" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A66" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D66" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E66" s="12"/>
+    </row>
+    <row r="67" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D67" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A68" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D68" s="10" t="s">
+        <v>80</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Gestion du planning terminé - correction de bugs
</commit_message>
<xml_diff>
--- a/Documentation/Tests unitaire/Tests unitaires.xlsx
+++ b/Documentation/Tests unitaire/Tests unitaires.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="95">
   <si>
     <t>Comportement Observé</t>
   </si>
@@ -126,12 +126,6 @@
     <t>Voir date arrivée</t>
   </si>
   <si>
-    <t xml:space="preserve">Lorsque je clique sur le bouton  :                                           Si aucune ligne n'a été sélectionnée, message d'avertissement                                                                                   Si la date de départ est celle du jour, message de confirmation pour être sûr que c'est bien la date voulue                                                                                                         Si l'heure de départ est à 0:0, message de confimration pour être sûr que c'est bien l'heure voulue                                                                                                        Si tous les champs sont renseignés, enable le bouton ajouter                                                                                            </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Si aucune ligne n'a été sélectionnée, message d'avertissement                                                                                   Si la date de départ est celle du jour, message de confirmation pour être sûr que c'est bien la date voulue                                                                                                         Si l'heure de départ est à 0:0, message de confimration pour être sûr que c'est bien l'heure voulue                                                                                                        Si tous les champs sont renseignés, enable le bouton ajouter       </t>
-  </si>
-  <si>
     <t>"Modification d'un champ"</t>
   </si>
   <si>
@@ -267,11 +261,59 @@
     <t xml:space="preserve">Si la date de début précède le jour même, message d'avertissement                                                                                         Si la date de fin précède la date de début, message d'avertissement                                                                                Si le nombre de jours que l'on veut ajouter dépasse le nombre de jours de vacances restant au pilote, message d'avertissement                                                               Si la date de débout ou la date de fin correspondent a une date de vacances deja existante du pilote, message d'avertissement                                                                      Si le pilote est en train de travailler pendant la periode de vacances, message d'avertissement                                                     Si la date de début et la date de fin sont "correctes", les vacances sont ajoutées dans la base de données, message d'avertissement                                                                               </t>
   </si>
   <si>
-    <t>OK, SAUF CAS SPECIFIQUE</t>
+    <t>Lorsque je clique sur ajouter si : un ou des champs ne sont pas remplis  -&gt; message d'avertissement; un champ ne contient pas les caractères adaptés à ce champ -&gt; message d'avertissement; le nom ou le prénom dépasse les 45 caractères -&gt; messages d'avertissement; si les heures de vols commencent par 0 -&gt; message d'avertissement.                                            Si tous les champs sont remplis correctement un pilote est ajouté dans la base de données</t>
+  </si>
+  <si>
+    <t>Lorsque je clique sur ajouter si: un ou des champs ne sont pas remplis -&gt; message d'avertissement, le champ distance ne contient pas que des chiffres ou commence par 0 -&gt; avertissement; le lieu d'arrivée et le meme que le lieu de départ -&gt; avertissement     Si la ligne que l'on veut ajouter existe deja, message d'avertissement</t>
+  </si>
+  <si>
+    <t>Lorsque je clique sur le bouton, un vol est ajouté dans la base de données et un message averti l'utilisateur que le vol a été ajouté                                                Si le vol existe déjà, message d'avertissement</t>
+  </si>
+  <si>
+    <t>Génération du planning</t>
+  </si>
+  <si>
+    <t>Générer planing</t>
+  </si>
+  <si>
+    <t>Si aucune ligne n'est sélectionnée dans le DataGridView, message d'avertissement                               Si toutes les lignes sont sélectionnées dans le DataGridView, message d'avertissement                              Si une seule ligne est sélectionnée, le formualire frmFlightAssignment s'ouvre</t>
+  </si>
+  <si>
+    <t>Si aucune ligne n'est sélectionnée dans le DataGridView, message d'avertissement                               Si toutes les lignes sont sélectionnées dans le DataGridView, message d'avertissement                              Si aucun mois est sélectionné dans cboMonth, message d'avertissement                                                                    Si une seule ligne est sélectionnée et un mois est sélectionné, crée un dossier (si il n'existe pas) planificationVolsAeriens, puis dans le dossier crée un autre dossier "idPilotPilotNamePilotFirstName", puis dans le dossier crée un dossier "Année" (ex: 2018), puis dans le dossier crée un fichier csv "AnnéeMois" (ex 201805) contenant pour chaque jour du mois l'activité du pilote</t>
+  </si>
+  <si>
+    <t>Si aucune ligne n'est sélectionnée dans le DataGridView, message d'avertissement                                                                              Si toutes les lignes sont sélectionnées dans le DataGridView, message d'avertissement                                                  Si aucun mois est sélectionné dans cboMonth, message d'avertissement                                                                                              Si une seule ligne est sélectionnée et un mois est sélectionné, crée les dossiers et le fichier csv</t>
+  </si>
+  <si>
+    <t>ficher.csv</t>
+  </si>
+  <si>
+    <t>Pour chaque jour du mois, l'activité du pilote est notée. Si il est en vacance "Vacation", si il est congé "Free Day", si il travaille "Nom du vol  dateDarrivée"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lorsque je clique sur le bouton  :                                           Si aucune ligne n'a été sélectionnée, message d'avertissement                                                                                   Si la date de départ est celle du jour, message de confirmation pour être sûr que c'est bien la date voulue                                                                                                         Si l'heure de départ est à 0:0, message de confimration pour être sûr que c'est bien l'heure voulue                                                                                                        Si tous les champs sont renseignés, enable le bouton ajouter, affiche la date d'arrivée                                                                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Si aucune ligne n'a été sélectionnée, message d'avertissement                                                                                   Si la date de départ est celle du jour, message de confirmation pour être sûr que c'est bien la date voulue                                                                                                         Si l'heure de départ est à 0:0, message de confimration pour être sûr que c'est bien l'heure voulue                                                                                                        Si tous les champs sont renseignés, enable le bouton ajouter, la date d'arrivée est affichée correctement  </t>
+  </si>
+  <si>
+    <t>un vol est ajouté dans la base de données et un message averti l'utilisateur que le vol a été ajouté                                        Si le vol existe déjà, l'utilisateur en est averti</t>
+  </si>
+  <si>
+    <t>Si le lieu de départ et/ou le lieu d'arrivée ne sont pas sélectionnés, message d'avertissement                                                       Si le lieu de départ correspond au lieu d'arrivée, message d'avertissement                                                                                                     Si la distance n'est pas rentrée, message d'avertissement    Si la distance commence par 0, message d'avertissement    Si la ligne existe deja, message d'avertissement                             Si tous les champs sont remplis correctement deux lignes sont crées (Ligne allé = ArrivalAirport-DepartureAirport, ligne retour DepartureAirport-ArrivalAirport)</t>
   </si>
   <si>
     <r>
       <t xml:space="preserve">Si la date de début précède le jour même, message d'avertissement                                                                                         Si la date de fin précède la date de début, message d'avertissement                                                                                    Si le nombre de jours que l'on veut ajouter dépasse le nombre de jours de vacances restant au pilote, message d'avertissement                                                                                    Si la date de débout ou la date de fin correspondent a une date de vacances deja existante du pilote, message d'avertissement                                                                                                  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Si le pilote est en train de travailler pendant la periode de vacances, message d'avertissement  </t>
     </r>
     <r>
       <rPr>
@@ -281,7 +323,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Si le pilote est en train de travailler pendant la periode de vacances, les vacances sont quand même ajoutées   </t>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
@@ -293,24 +335,6 @@
       </rPr>
       <t xml:space="preserve">                                                                                   Si la date de début et la date de fin sont "correctes", les vacances sont ajoutées dans la base de données, message d'avertissement</t>
     </r>
-  </si>
-  <si>
-    <t>Lorsque je clique sur ajouter si : un ou des champs ne sont pas remplis  -&gt; message d'avertissement; un champ ne contient pas les caractères adaptés à ce champ -&gt; message d'avertissement; le nom ou le prénom dépasse les 45 caractères -&gt; messages d'avertissement; si les heures de vols commencent par 0 -&gt; message d'avertissement.                                            Si tous les champs sont remplis correctement un pilote est ajouté dans la base de données</t>
-  </si>
-  <si>
-    <t>Lorsque je clique sur ajouter si: un ou des champs ne sont pas remplis -&gt; message d'avertissement, le champ distance ne contient pas que des chiffres ou commence par 0 -&gt; avertissement; le lieu d'arrivée et le meme que le lieu de départ -&gt; avertissement     Si la ligne que l'on veut ajouter existe deja, message d'avertissement</t>
-  </si>
-  <si>
-    <t>Si le lieu de départ et/ou le lieu d'arrivée ne sont pas sélectionnés, message d'avertissement                                                       Si le lieu de départ correspond au lieu d'arrivée, message d'avertissement                                                                                                     Si la distance n'est pas rentrée, message d'avertissement    Si la distance commence par 0, message d'avertissement    Il n'y a pas de vérification si la ligne existe deja                              Si tous les champs sont remplis correctement deux lignes sont crées (Ligne allé = ArrivalAirport-DepartureAirport, ligne retour DepartureAirport-ArrivalAirport)</t>
-  </si>
-  <si>
-    <t>Lorsque je clique sur le bouton, un vol est ajouté dans la base de données et un message averti l'utilisateur que le vol a été ajouté                                                Si le vol existe déjà, message d'avertissement</t>
-  </si>
-  <si>
-    <t>un vol est ajouté dans la base de données et un message averti l'utilisateur que le vol a été ajouté                                        Il n'y a pas de vérification si le vol existe déjà ou pas</t>
-  </si>
-  <si>
-    <t>OK, sauf cas spécifique</t>
   </si>
 </sst>
 </file>
@@ -347,7 +371,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -384,12 +408,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -418,7 +436,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -448,10 +466,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -734,10 +749,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E68"/>
+  <dimension ref="A1:E77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="A71" sqref="A71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -829,7 +844,7 @@
         <v>13</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>14</v>
@@ -915,13 +930,13 @@
         <v>13</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>82</v>
+        <v>93</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -990,24 +1005,24 @@
         <v>34</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>35</v>
+        <v>90</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D25" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D25" s="13" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>2</v>
@@ -1018,18 +1033,18 @@
         <v>13</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="D27" s="13" t="s">
-        <v>89</v>
+        <v>92</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1048,13 +1063,13 @@
     </row>
     <row r="33" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>2</v>
@@ -1062,7 +1077,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1081,13 +1096,13 @@
     </row>
     <row r="39" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>2</v>
@@ -1095,7 +1110,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1114,13 +1129,13 @@
     </row>
     <row r="44" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D44" s="5" t="s">
         <v>2</v>
@@ -1128,7 +1143,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1147,13 +1162,13 @@
     </row>
     <row r="49" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D49" s="5" t="s">
         <v>2</v>
@@ -1161,16 +1176,16 @@
     </row>
     <row r="50" spans="1:4" ht="225" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D50" s="14" t="s">
-        <v>82</v>
+        <v>94</v>
+      </c>
+      <c r="D50" s="13" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1187,7 +1202,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1206,13 +1221,13 @@
     </row>
     <row r="55" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C55" s="6" t="s">
         <v>55</v>
-      </c>
-      <c r="B55" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C55" s="6" t="s">
-        <v>57</v>
       </c>
       <c r="D55" s="5" t="s">
         <v>2</v>
@@ -1220,13 +1235,13 @@
     </row>
     <row r="56" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D56" s="5" t="s">
         <v>2</v>
@@ -1237,7 +1252,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -1256,95 +1271,142 @@
     </row>
     <row r="62" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D62" s="5" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="3" t="s">
+      <c r="A63" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A64" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B64" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D64" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A65" s="6" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A64" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B64" s="3" t="s">
+      <c r="B65" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="C64" s="6" t="s">
+      <c r="C65" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D65" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A66" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D66" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E66" s="12"/>
+    </row>
+    <row r="67" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A67" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D67" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A68" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D68" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="D64" s="11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A65" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B65" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="C65" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D65" s="9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A66" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C66" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="D66" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E66" s="12"/>
-    </row>
-    <row r="67" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A67" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C67" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D67" s="9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A68" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C68" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="D68" s="10" t="s">
-        <v>80</v>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="225" x14ac:dyDescent="0.25">
+      <c r="A76" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B76" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C76" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A77" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B77" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>